<commit_message>
fix import file, build profile page, update present kpi, build scroll into view target
</commit_message>
<xml_diff>
--- a/kpi/public/template.xlsx
+++ b/kpi/public/template.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AECC910-1748-4219-A562-3DCEDBE52E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB157C73-8433-4E8D-90E6-FF606547B757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Mục tiêu</t>
   </si>
@@ -58,12 +71,6 @@
     <t>Cố lên, cố lên, anh cố lên!!!</t>
   </si>
   <si>
-    <t>Số giờ lên lớp</t>
-  </si>
-  <si>
-    <t>hihihaa</t>
-  </si>
-  <si>
     <t>Giờ</t>
   </si>
   <si>
@@ -76,18 +83,15 @@
     <t>Lên lớp 234</t>
   </si>
   <si>
+    <t>Buổi</t>
+  </si>
+  <si>
     <t>Phục vụ</t>
   </si>
   <si>
     <t>Bla bla blo blo</t>
   </si>
   <si>
-    <t>Số lần tham gia hội thảo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bla bla </t>
-  </si>
-  <si>
     <t>Lần</t>
   </si>
   <si>
@@ -97,7 +101,37 @@
     <t>Hội thảo ở C2</t>
   </si>
   <si>
+    <t>Đi với soict</t>
+  </si>
+  <si>
+    <t>Đi với team</t>
+  </si>
+  <si>
     <t>Tiến độ</t>
+  </si>
+  <si>
+    <t>Tiêu chí giảng dạy 1</t>
+  </si>
+  <si>
+    <t>Tiêu chí giảng dạy 2</t>
+  </si>
+  <si>
+    <t>Tiêu chí phục vụ 1</t>
+  </si>
+  <si>
+    <t>Tiêu chí phục vụ 2</t>
+  </si>
+  <si>
+    <t>Mô tả tc 1</t>
+  </si>
+  <si>
+    <t>mô tả tc 2</t>
+  </si>
+  <si>
+    <t>Mô tả tiêu chí 4</t>
+  </si>
+  <si>
+    <t>Mô tả tiêu chí 3</t>
   </si>
 </sst>
 </file>
@@ -158,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -202,6 +236,17 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -211,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -231,7 +276,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,10 +499,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -505,7 +554,7 @@
         <v>7</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>8</v>
@@ -525,31 +574,31 @@
         <v>40</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F2" s="6">
         <v>40</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H2" s="6">
         <v>40</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K2" s="4">
         <v>20</v>
       </c>
       <c r="L2" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M2" s="5">
         <v>45429</v>
@@ -559,25 +608,25 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K3" s="4">
         <v>20</v>
       </c>
-      <c r="L3" s="4">
-        <v>0</v>
+      <c r="L3">
+        <v>6</v>
       </c>
       <c r="M3" s="5">
         <v>45430</v>
@@ -587,95 +636,237 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="F4" s="6">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6">
+        <v>60</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4">
         <v>5</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="6">
-        <v>70</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="4">
-        <v>3</v>
-      </c>
       <c r="L4" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M4" s="5">
-        <v>45433</v>
+        <v>45431</v>
       </c>
       <c r="N4" s="5">
-        <v>45465</v>
+        <v>45463</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K5" s="4">
+        <v>5</v>
+      </c>
+      <c r="L5" s="4">
+        <v>4</v>
+      </c>
+      <c r="M5" s="5">
+        <v>45432</v>
+      </c>
+      <c r="N5" s="5">
+        <v>45464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6">
+        <v>30</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="6">
+        <v>70</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="4">
+        <v>3</v>
+      </c>
+      <c r="L6" s="4">
         <v>2</v>
       </c>
-      <c r="L5" s="4">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5">
+      <c r="M6" s="5">
+        <v>45433</v>
+      </c>
+      <c r="N6" s="5">
+        <v>45465</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+      <c r="M7" s="5">
         <v>45434</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N7" s="5">
         <v>45466</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="6">
+        <v>3</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="6">
+        <v>30</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="4">
+        <v>2</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+      <c r="M8" s="5">
+        <v>45435</v>
+      </c>
+      <c r="N8" s="5">
+        <v>45467</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
+      <c r="M9" s="5">
+        <v>45436</v>
+      </c>
+      <c r="N9" s="5">
+        <v>45468</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="26">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>